<commit_message>
Hour index for Extraction and Trade
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2125F8E9-F139-3E4E-8290-2C86BA2AB99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217BDA04-D6FA-1F4F-B31E-B09E21626905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3873" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="109">
   <si>
     <t>Type</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>input_share_min</t>
+  </si>
+  <si>
+    <t>flow_in_share_max</t>
   </si>
 </sst>
 </file>
@@ -4775,7 +4778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+    <sheetView topLeftCell="A255" workbookViewId="0">
       <selection activeCell="G273" sqref="G273"/>
     </sheetView>
   </sheetViews>
@@ -15322,8 +15325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView topLeftCell="A257" workbookViewId="0">
-      <selection activeCell="F315" sqref="F315"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23998,10 +24001,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24521,21 +24524,34 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="7:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="G54" s="3"/>
+    <row r="55" spans="7:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -29607,9 +29623,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -34377,10 +34399,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G322"/>
+  <dimension ref="A1:G324"/>
   <sheetViews>
-    <sheetView topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="G364" sqref="G364"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B322" sqref="B322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39586,12 +39608,18 @@
         <v>5</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
+      <c r="E310">
+        <v>0</v>
+      </c>
       <c r="F310">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.2">
@@ -39599,12 +39627,12 @@
         <v>5</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
       <c r="F311">
-        <v>8.7611111118119993</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.2">
@@ -39612,18 +39640,12 @@
         <v>5</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
-      <c r="E312">
-        <v>0</v>
-      </c>
       <c r="F312">
-        <v>257614.48541000011</v>
-      </c>
-      <c r="G312">
-        <v>0</v>
+        <v>8.7611111118119993</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.2">
@@ -39631,12 +39653,18 @@
         <v>5</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
+      <c r="E313">
+        <v>0</v>
+      </c>
       <c r="F313">
-        <v>8.3000000000000007</v>
+        <v>257614.48541000011</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.2">
@@ -39644,12 +39672,12 @@
         <v>5</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
       <c r="F314">
-        <v>30</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.2">
@@ -39657,15 +39685,12 @@
         <v>5</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
-      <c r="E315">
-        <v>4.3938888892404009</v>
-      </c>
-      <c r="G315">
-        <v>4.3938888892404009</v>
+      <c r="F315">
+        <v>30</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.2">
@@ -39673,27 +39698,28 @@
         <v>5</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
-      <c r="F316">
-        <v>8</v>
+      <c r="E316">
+        <v>4.3938888892404009</v>
+      </c>
+      <c r="G316">
+        <v>4.3938888892404009</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C317" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C317" s="2"/>
       <c r="D317" s="2"/>
       <c r="F317">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.2">
@@ -39701,14 +39727,14 @@
         <v>57</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D318" s="2"/>
       <c r="F318">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.2">
@@ -39716,7 +39742,7 @@
         <v>57</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>47</v>
@@ -39731,14 +39757,14 @@
         <v>57</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D320" s="2"/>
-      <c r="E320">
-        <v>1</v>
+      <c r="F320">
+        <v>0.4</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.2">
@@ -39746,14 +39772,14 @@
         <v>57</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D321" s="2"/>
       <c r="F321">
-        <v>1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.2">
@@ -39764,10 +39790,40 @@
         <v>59</v>
       </c>
       <c r="C322" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D322" s="2"/>
+      <c r="E322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A323" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D323" s="2"/>
+      <c r="F323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A324" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C324" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D322" s="2"/>
-      <c r="G322">
+      <c r="D324" s="2"/>
+      <c r="G324">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hour index for Storage (+fixes) and documentation.
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217BDA04-D6FA-1F4F-B31E-B09E21626905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8567E9-3894-0449-A5B5-EF3EA302BA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -4778,8 +4778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K328"/>
   <sheetViews>
-    <sheetView topLeftCell="A255" workbookViewId="0">
-      <selection activeCell="G273" sqref="G273"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E205" sqref="E205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29623,8 +29623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="H302" sqref="H302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34281,7 +34281,7 @@
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
       <c r="E311">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
@@ -34401,7 +34401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B322" sqref="B322"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Representative day fix complete.
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8567E9-3894-0449-A5B5-EF3EA302BA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C719CE-B0F3-8640-AC9D-8EBD9E70D335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -4364,9 +4364,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
@@ -4535,9 +4552,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
@@ -15325,8 +15359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15335,6 +15369,10 @@
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -22967,9 +23005,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -24003,8 +24047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29623,7 +29667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+    <sheetView topLeftCell="A217" workbookViewId="0">
       <selection activeCell="H302" sqref="H302"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Renamed sector to modules
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C719CE-B0F3-8640-AC9D-8EBD9E70D335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893F96C5-785F-414A-9437-53545A714F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3878" uniqueCount="109">
   <si>
     <t>Type</t>
   </si>
@@ -360,9 +360,6 @@
     <t>enable_import</t>
   </si>
   <si>
-    <t>max_share_at_out_flow</t>
-  </si>
-  <si>
     <t>flow_out_share_max</t>
   </si>
   <si>
@@ -370,6 +367,9 @@
   </si>
   <si>
     <t>flow_in_share_max</t>
+  </si>
+  <si>
+    <t>revenue</t>
   </si>
 </sst>
 </file>
@@ -768,9 +768,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -22870,7 +22879,7 @@
         <v>57</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>64</v>
@@ -24047,7 +24056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -34443,10 +34452,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G324"/>
+  <dimension ref="A1:K323"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B322" sqref="B322"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="J317" sqref="J317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36988,7 +36997,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>8</v>
       </c>
@@ -37003,7 +37012,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>8</v>
       </c>
@@ -37018,7 +37027,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>8</v>
       </c>
@@ -37033,7 +37042,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>8</v>
       </c>
@@ -37048,7 +37057,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>8</v>
       </c>
@@ -37063,7 +37072,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>8</v>
       </c>
@@ -37078,7 +37087,7 @@
         <v>4079794.5519329761</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>8</v>
       </c>
@@ -37092,8 +37101,11 @@
       <c r="F151">
         <v>4079794.5519329761</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I151" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>8</v>
       </c>
@@ -37113,8 +37125,15 @@
       <c r="G152">
         <v>13598251.985717461</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I152">
+        <v>72868380.462301552</v>
+      </c>
+      <c r="K152">
+        <f>F152-I152</f>
+        <v>608047.2334971875</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>8</v>
       </c>
@@ -37134,8 +37153,15 @@
       <c r="G153">
         <v>12866478.36734629</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I153">
+        <v>69443665.369608507</v>
+      </c>
+      <c r="K153">
+        <f t="shared" ref="K153:K181" si="0">F153-I153</f>
+        <v>579469.83786386251</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>8</v>
       </c>
@@ -37155,8 +37181,15 @@
       <c r="G154">
         <v>11131658.94646023</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I154">
+        <v>72462612.675985932</v>
+      </c>
+      <c r="K154">
+        <f t="shared" si="0"/>
+        <v>536241.98569744825</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>8</v>
       </c>
@@ -37176,8 +37209,15 @@
       <c r="G155">
         <v>9705918.5024779923</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I155">
+        <v>65572779.847597606</v>
+      </c>
+      <c r="K155">
+        <f t="shared" si="0"/>
+        <v>820739.668711707</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>8</v>
       </c>
@@ -37197,8 +37237,15 @@
       <c r="G156">
         <v>9238501.0401054472</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I156">
+        <v>60048782.662673987</v>
+      </c>
+      <c r="K156">
+        <f t="shared" si="0"/>
+        <v>1003489.0150847957</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>8</v>
       </c>
@@ -37218,8 +37265,15 @@
       <c r="G157">
         <v>10110283.82031228</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I157">
+        <v>54624821.773283303</v>
+      </c>
+      <c r="K157">
+        <f t="shared" si="0"/>
+        <v>2860037.4784208685</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>8</v>
       </c>
@@ -37239,8 +37293,15 @@
       <c r="G158">
         <v>10361908.70683069</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I158">
+        <v>52817675.119184971</v>
+      </c>
+      <c r="K158">
+        <f t="shared" si="0"/>
+        <v>4829482.6306366473</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>8</v>
       </c>
@@ -37260,8 +37321,15 @@
       <c r="G159">
         <v>10351202.98512923</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I159">
+        <v>54848741.10607145</v>
+      </c>
+      <c r="K159">
+        <f t="shared" si="0"/>
+        <v>4887111.6891271099</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>8</v>
       </c>
@@ -37281,8 +37349,15 @@
       <c r="G160">
         <v>10336403.519480599</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I160">
+        <v>52996779.672382981</v>
+      </c>
+      <c r="K160">
+        <f t="shared" si="0"/>
+        <v>4995925.6855564564</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>8</v>
       </c>
@@ -37302,8 +37377,15 @@
       <c r="G161">
         <v>9994162.7212954368</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I161">
+        <v>50055780.142816558</v>
+      </c>
+      <c r="K161">
+        <f t="shared" si="0"/>
+        <v>4702567.395492591</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>8</v>
       </c>
@@ -37323,8 +37405,15 @@
       <c r="G162">
         <v>12100025.433453809</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I162">
+        <v>47283191.208029032</v>
+      </c>
+      <c r="K162">
+        <f t="shared" si="0"/>
+        <v>2950471.1313810274</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>8</v>
       </c>
@@ -37344,8 +37433,15 @@
       <c r="G163">
         <v>13675155.73827382</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I163">
+        <v>46753372.633913897</v>
+      </c>
+      <c r="K163">
+        <f t="shared" si="0"/>
+        <v>4501101.0920848697</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>8</v>
       </c>
@@ -37365,8 +37461,15 @@
       <c r="G164">
         <v>11371821.596399689</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I164">
+        <v>44005098.906308956</v>
+      </c>
+      <c r="K164">
+        <f t="shared" si="0"/>
+        <v>-12390124.428917807</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>8</v>
       </c>
@@ -37386,8 +37489,15 @@
       <c r="G165">
         <v>11848595.448392419</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I165">
+        <v>46981029.422235534</v>
+      </c>
+      <c r="K165">
+        <f t="shared" si="0"/>
+        <v>-15161805.214145783</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>8</v>
       </c>
@@ -37407,8 +37517,15 @@
       <c r="G166">
         <v>15960391.11326655</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I166">
+        <v>46530664.187545687</v>
+      </c>
+      <c r="K166">
+        <f t="shared" si="0"/>
+        <v>-13292299.353463788</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>8</v>
       </c>
@@ -37428,8 +37545,15 @@
       <c r="G167">
         <v>15823946.27520548</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I167">
+        <v>49665137.464181773</v>
+      </c>
+      <c r="K167">
+        <f t="shared" si="0"/>
+        <v>-5359225.4309117869</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>8</v>
       </c>
@@ -37449,8 +37573,15 @@
       <c r="G168">
         <v>15766247.29546619</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I168">
+        <v>55492492.594764411</v>
+      </c>
+      <c r="K168">
+        <f t="shared" si="0"/>
+        <v>-438887.16274977475</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>8</v>
       </c>
@@ -37470,8 +37601,15 @@
       <c r="G169">
         <v>19335684.265480291</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I169">
+        <v>61889368.045708351</v>
+      </c>
+      <c r="K169">
+        <f t="shared" si="0"/>
+        <v>-8176174.6279377714</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>8</v>
       </c>
@@ -37491,8 +37629,15 @@
       <c r="G170">
         <v>29760133.18130257</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I170">
+        <v>52359558.228543051</v>
+      </c>
+      <c r="K170">
+        <f t="shared" si="0"/>
+        <v>6961707.3844585493</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>8</v>
       </c>
@@ -37512,8 +37657,15 @@
       <c r="G171">
         <v>18969216.577792492</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I171">
+        <v>52958723.926128447</v>
+      </c>
+      <c r="K171">
+        <f t="shared" si="0"/>
+        <v>903278.93179946393</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>8</v>
       </c>
@@ -37533,8 +37685,15 @@
       <c r="G172">
         <v>20414586.94241805</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I172">
+        <v>46805215.284266718</v>
+      </c>
+      <c r="K172">
+        <f t="shared" si="0"/>
+        <v>2479640.2006545588</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>8</v>
       </c>
@@ -37554,8 +37713,15 @@
       <c r="G173">
         <v>22459800.84431199</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I173">
+        <v>44090948.411104701</v>
+      </c>
+      <c r="K173">
+        <f t="shared" si="0"/>
+        <v>5312481.2598892152</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>8</v>
       </c>
@@ -37575,8 +37741,15 @@
       <c r="G174">
         <v>18028289.74834403</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I174">
+        <v>44826475.455966637</v>
+      </c>
+      <c r="K174">
+        <f t="shared" si="0"/>
+        <v>8513989.6805758849</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>8</v>
       </c>
@@ -37596,8 +37769,15 @@
       <c r="G175">
         <v>14438258.730778299</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I175">
+        <v>44028056.463124707</v>
+      </c>
+      <c r="K175">
+        <f t="shared" si="0"/>
+        <v>6211232.4630410746</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>8</v>
       </c>
@@ -37617,8 +37797,15 @@
       <c r="G176">
         <v>13044758.58774277</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I176">
+        <v>41580608.14573615</v>
+      </c>
+      <c r="K176">
+        <f t="shared" si="0"/>
+        <v>1790892.6618613899</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>8</v>
       </c>
@@ -37638,8 +37825,15 @@
       <c r="G177">
         <v>12194657.85763051</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I177">
+        <v>35296943.933920287</v>
+      </c>
+      <c r="K177">
+        <f t="shared" si="0"/>
+        <v>2876103.876196146</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>8</v>
       </c>
@@ -37659,8 +37853,15 @@
       <c r="G178">
         <v>11560902.823346499</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I178">
+        <v>33913535.910064884</v>
+      </c>
+      <c r="K178">
+        <f t="shared" si="0"/>
+        <v>2524141.4880312458</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>8</v>
       </c>
@@ -37680,8 +37881,15 @@
       <c r="G179">
         <v>12323761.39009171</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I179">
+        <v>33308730.000723761</v>
+      </c>
+      <c r="K179">
+        <f t="shared" si="0"/>
+        <v>-1220146.0763105005</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>8</v>
       </c>
@@ -37701,8 +37909,15 @@
       <c r="G180">
         <v>14729662.633355061</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I180">
+        <v>34893956.186830908</v>
+      </c>
+      <c r="K180">
+        <f t="shared" si="0"/>
+        <v>-803649.80816623569</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>8</v>
       </c>
@@ -37722,8 +37937,15 @@
       <c r="G181">
         <v>12212183.227296</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I181">
+        <v>37300000</v>
+      </c>
+      <c r="K181">
+        <f t="shared" si="0"/>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>8</v>
       </c>
@@ -37738,7 +37960,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>8</v>
       </c>
@@ -37753,7 +37975,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>8</v>
       </c>
@@ -37768,7 +37990,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>8</v>
       </c>
@@ -37783,7 +38005,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>8</v>
       </c>
@@ -37798,7 +38020,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>8</v>
       </c>
@@ -37813,7 +38035,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>8</v>
       </c>
@@ -37828,7 +38050,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>8</v>
       </c>
@@ -37843,7 +38065,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>8</v>
       </c>
@@ -37858,7 +38080,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>8</v>
       </c>
@@ -37873,7 +38095,7 @@
         <v>583725344.15728891</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>8</v>
       </c>
@@ -39749,6 +39971,9 @@
       <c r="E316">
         <v>4.3938888892404009</v>
       </c>
+      <c r="F316">
+        <v>30</v>
+      </c>
       <c r="G316">
         <v>4.3938888892404009</v>
       </c>
@@ -39801,7 +40026,7 @@
         <v>57</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>47</v>
@@ -39816,14 +40041,14 @@
         <v>57</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D321" s="2"/>
-      <c r="F321">
-        <v>0.4</v>
+      <c r="E321">
+        <v>1</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.2">
@@ -39834,10 +40059,10 @@
         <v>59</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D322" s="2"/>
-      <c r="E322">
+      <c r="F322">
         <v>1</v>
       </c>
     </row>
@@ -39849,25 +40074,10 @@
         <v>59</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D323" s="2"/>
-      <c r="F323">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A324" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C324" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D324" s="2"/>
-      <c r="G324">
+      <c r="G323">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed Year Slicing. Other fixes: - Better plotting Extras: - Corrected headers - Project license is now Apache 2.0
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893F96C5-785F-414A-9437-53545A714F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69779A3E-F297-0D4A-845A-BDB519096551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15368,8 +15368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="B212" sqref="B212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21187,12 +21187,6 @@
       <c r="F242">
         <v>1</v>
       </c>
-      <c r="G242">
-        <v>1</v>
-      </c>
-      <c r="H242">
-        <v>1</v>
-      </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
@@ -21211,12 +21205,6 @@
       <c r="F243">
         <v>0.48193489699999997</v>
       </c>
-      <c r="G243">
-        <v>0.3</v>
-      </c>
-      <c r="H243">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
@@ -21235,12 +21223,6 @@
       <c r="F244">
         <v>0.52774263899999996</v>
       </c>
-      <c r="G244">
-        <v>0.3</v>
-      </c>
-      <c r="H244">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
@@ -21259,12 +21241,6 @@
       <c r="F245">
         <v>0.53578760199999997</v>
       </c>
-      <c r="G245">
-        <v>0.3</v>
-      </c>
-      <c r="H245">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
@@ -21283,12 +21259,6 @@
       <c r="F246">
         <v>0.57528420899999999</v>
       </c>
-      <c r="G246">
-        <v>0.3</v>
-      </c>
-      <c r="H246">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
@@ -21307,12 +21277,6 @@
       <c r="F247">
         <v>0.55995716799999995</v>
       </c>
-      <c r="G247">
-        <v>0.3</v>
-      </c>
-      <c r="H247">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
@@ -21331,12 +21295,6 @@
       <c r="F248">
         <v>0.461516749</v>
       </c>
-      <c r="G248">
-        <v>0.3</v>
-      </c>
-      <c r="H248">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
@@ -21355,12 +21313,6 @@
       <c r="F249">
         <v>0.49615836000000002</v>
       </c>
-      <c r="G249">
-        <v>0.3</v>
-      </c>
-      <c r="H249">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
@@ -21379,12 +21331,6 @@
       <c r="F250">
         <v>0.505308337</v>
       </c>
-      <c r="G250">
-        <v>0.3</v>
-      </c>
-      <c r="H250">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
@@ -21403,12 +21349,6 @@
       <c r="F251">
         <v>0.56182886099999996</v>
       </c>
-      <c r="G251">
-        <v>0.3</v>
-      </c>
-      <c r="H251">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
@@ -21427,12 +21367,6 @@
       <c r="F252">
         <v>0.59309409700000004</v>
       </c>
-      <c r="G252">
-        <v>0.3</v>
-      </c>
-      <c r="H252">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
@@ -21451,12 +21385,6 @@
       <c r="F253">
         <v>0.58312801800000003</v>
       </c>
-      <c r="G253">
-        <v>0.3</v>
-      </c>
-      <c r="H253">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
@@ -21475,12 +21403,6 @@
       <c r="F254">
         <v>0.57898886400000005</v>
       </c>
-      <c r="G254">
-        <v>0.3</v>
-      </c>
-      <c r="H254">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
@@ -21499,12 +21421,6 @@
       <c r="F255">
         <v>0.50583095199999994</v>
       </c>
-      <c r="G255">
-        <v>0.3</v>
-      </c>
-      <c r="H255">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
@@ -21523,12 +21439,6 @@
       <c r="F256">
         <v>0.52688807900000001</v>
       </c>
-      <c r="G256">
-        <v>0.3</v>
-      </c>
-      <c r="H256">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
@@ -21547,12 +21457,6 @@
       <c r="F257">
         <v>0.49269077900000002</v>
       </c>
-      <c r="G257">
-        <v>0.3</v>
-      </c>
-      <c r="H257">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
@@ -21571,12 +21475,6 @@
       <c r="F258">
         <v>0.496104922</v>
       </c>
-      <c r="G258">
-        <v>0.3</v>
-      </c>
-      <c r="H258">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
@@ -21595,12 +21493,6 @@
       <c r="F259">
         <v>0.51893597300000005</v>
       </c>
-      <c r="G259">
-        <v>0.3</v>
-      </c>
-      <c r="H259">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
@@ -21619,12 +21511,6 @@
       <c r="F260">
         <v>0.52074867999999996</v>
       </c>
-      <c r="G260">
-        <v>0.3</v>
-      </c>
-      <c r="H260">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
@@ -21643,12 +21529,6 @@
       <c r="F261">
         <v>0.50277245800000003</v>
       </c>
-      <c r="G261">
-        <v>0.3</v>
-      </c>
-      <c r="H261">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
@@ -21667,12 +21547,6 @@
       <c r="F262">
         <v>0.485641975</v>
       </c>
-      <c r="G262">
-        <v>0.3</v>
-      </c>
-      <c r="H262">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
@@ -21691,12 +21565,6 @@
       <c r="F263">
         <v>0.44142679099999999</v>
       </c>
-      <c r="G263">
-        <v>0.3</v>
-      </c>
-      <c r="H263">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
@@ -21715,12 +21583,6 @@
       <c r="F264">
         <v>0.53012915599999999</v>
       </c>
-      <c r="G264">
-        <v>0.3</v>
-      </c>
-      <c r="H264">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
@@ -21739,12 +21601,6 @@
       <c r="F265">
         <v>0.52608195199999996</v>
       </c>
-      <c r="G265">
-        <v>0.3</v>
-      </c>
-      <c r="H265">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
@@ -21763,12 +21619,6 @@
       <c r="F266">
         <v>0.50552529199999996</v>
       </c>
-      <c r="G266">
-        <v>0.3</v>
-      </c>
-      <c r="H266">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
@@ -21787,12 +21637,6 @@
       <c r="F267">
         <v>0.480652774</v>
       </c>
-      <c r="G267">
-        <v>0.3</v>
-      </c>
-      <c r="H267">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
@@ -21811,12 +21655,6 @@
       <c r="F268">
         <v>0.47252149199999999</v>
       </c>
-      <c r="G268">
-        <v>0.3</v>
-      </c>
-      <c r="H268">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
@@ -21835,12 +21673,6 @@
       <c r="F269">
         <v>0.44910678799999998</v>
       </c>
-      <c r="G269">
-        <v>0.3</v>
-      </c>
-      <c r="H269">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
@@ -21859,12 +21691,6 @@
       <c r="F270">
         <v>0.46703340799999998</v>
       </c>
-      <c r="G270">
-        <v>0.3</v>
-      </c>
-      <c r="H270">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
@@ -21882,12 +21708,6 @@
       </c>
       <c r="F271">
         <v>0.48551606800000002</v>
-      </c>
-      <c r="G271">
-        <v>0.3</v>
-      </c>
-      <c r="H271">
-        <v>0.2</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.2">
@@ -29676,7 +29496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView topLeftCell="A217" workbookViewId="0">
+    <sheetView topLeftCell="A187" workbookViewId="0">
       <selection activeCell="H302" sqref="H302"/>
     </sheetView>
   </sheetViews>
@@ -34454,8 +34274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="J317" sqref="J317"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39955,9 +39775,6 @@
       </c>
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
-      <c r="F315">
-        <v>30</v>
-      </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">

</xml_diff>

<commit_message>
LF fix for hydro
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D8E215-624A-5A47-BD8E-B790BDC73A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C81865F-FDDB-7E42-8F3B-74C1F44D58EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country" sheetId="1" r:id="rId1"/>
@@ -4821,8 +4821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="M268" sqref="M268"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="G332" sqref="G332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15368,8 +15368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="E242" sqref="E242:F242"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="F202" sqref="F202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21722,10 +21722,10 @@
         <v>1990</v>
       </c>
       <c r="E272">
-        <v>0</v>
+        <v>0.23962008900000001</v>
       </c>
       <c r="F272">
-        <v>0</v>
+        <v>0.25941034499999999</v>
       </c>
       <c r="G272">
         <v>0.05</v>

</xml_diff>

<commit_message>
Improved graph plotting. - also some documentation fixes. - Fixed license text.
</commit_message>
<xml_diff>
--- a/data/cnf_files/test.xlsx
+++ b/data/cnf_files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/cnf_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C81865F-FDDB-7E42-8F3B-74C1F44D58EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48833EA-80A2-094B-B7D8-67E0A376D031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4821,14 +4821,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K328"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="G332" sqref="G332"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J272" sqref="J272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -13803,7 +13804,7 @@
         <v>0.2</v>
       </c>
       <c r="J272">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K272">
         <v>0.1</v>
@@ -13836,7 +13837,7 @@
         <v>0.2</v>
       </c>
       <c r="J273">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K273">
         <v>0.1</v>
@@ -13869,7 +13870,7 @@
         <v>0.2</v>
       </c>
       <c r="J274">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K274">
         <v>0.1</v>
@@ -13902,7 +13903,7 @@
         <v>0.2</v>
       </c>
       <c r="J275">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K275">
         <v>0.1</v>
@@ -13935,7 +13936,7 @@
         <v>0.2</v>
       </c>
       <c r="J276">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K276">
         <v>0.1</v>
@@ -13968,7 +13969,7 @@
         <v>0.2</v>
       </c>
       <c r="J277">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K277">
         <v>0.1</v>
@@ -14001,7 +14002,7 @@
         <v>0.2</v>
       </c>
       <c r="J278">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K278">
         <v>0.1</v>
@@ -14034,7 +14035,7 @@
         <v>0.2</v>
       </c>
       <c r="J279">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K279">
         <v>0.1</v>
@@ -14067,7 +14068,7 @@
         <v>0.2</v>
       </c>
       <c r="J280">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K280">
         <v>0.1</v>
@@ -14100,7 +14101,7 @@
         <v>0.2</v>
       </c>
       <c r="J281">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K281">
         <v>0.1</v>
@@ -14133,7 +14134,7 @@
         <v>0.2</v>
       </c>
       <c r="J282">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K282">
         <v>0.1</v>
@@ -14166,7 +14167,7 @@
         <v>0.2</v>
       </c>
       <c r="J283">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K283">
         <v>0.1</v>
@@ -14199,7 +14200,7 @@
         <v>0.2</v>
       </c>
       <c r="J284">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K284">
         <v>0.1</v>
@@ -14232,7 +14233,7 @@
         <v>0.2</v>
       </c>
       <c r="J285">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K285">
         <v>0.1</v>
@@ -14265,7 +14266,7 @@
         <v>0.2</v>
       </c>
       <c r="J286">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K286">
         <v>0.1</v>
@@ -14298,7 +14299,7 @@
         <v>0.2</v>
       </c>
       <c r="J287">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K287">
         <v>0.1</v>
@@ -14331,7 +14332,7 @@
         <v>0.2</v>
       </c>
       <c r="J288">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K288">
         <v>0.1</v>
@@ -14364,7 +14365,7 @@
         <v>0.2</v>
       </c>
       <c r="J289">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K289">
         <v>0.1</v>
@@ -14397,7 +14398,7 @@
         <v>0.2</v>
       </c>
       <c r="J290">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K290">
         <v>0.1</v>
@@ -14430,7 +14431,7 @@
         <v>0.2</v>
       </c>
       <c r="J291">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K291">
         <v>0.1</v>
@@ -14463,7 +14464,7 @@
         <v>0.2</v>
       </c>
       <c r="J292">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K292">
         <v>0.1</v>
@@ -14496,7 +14497,7 @@
         <v>0.2</v>
       </c>
       <c r="J293">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K293">
         <v>0.1</v>
@@ -14529,7 +14530,7 @@
         <v>0.2</v>
       </c>
       <c r="J294">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K294">
         <v>0.1</v>
@@ -14562,7 +14563,7 @@
         <v>0.2</v>
       </c>
       <c r="J295">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K295">
         <v>0.1</v>
@@ -14595,7 +14596,7 @@
         <v>0.2</v>
       </c>
       <c r="J296">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K296">
         <v>0.1</v>
@@ -14628,7 +14629,7 @@
         <v>0.2</v>
       </c>
       <c r="J297">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K297">
         <v>0.1</v>
@@ -14661,7 +14662,7 @@
         <v>0.2</v>
       </c>
       <c r="J298">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K298">
         <v>0.1</v>
@@ -14694,7 +14695,7 @@
         <v>0.2</v>
       </c>
       <c r="J299">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K299">
         <v>0.1</v>
@@ -14727,7 +14728,7 @@
         <v>0.2</v>
       </c>
       <c r="J300">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K300">
         <v>0.1</v>
@@ -14760,7 +14761,7 @@
         <v>0.2</v>
       </c>
       <c r="J301">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K301">
         <v>0.1</v>
@@ -15368,8 +15369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="F202" sqref="F202"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29496,8 +29497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="H302" sqref="H302"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34274,8 +34275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K323"/>
   <sheetViews>
-    <sheetView topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="G314" sqref="G314"/>
+    <sheetView topLeftCell="A296" workbookViewId="0">
+      <selection activeCell="F301" sqref="F301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>